<commit_message>
[Add] 30055 (include xlsx) [Modify] AI2.cs/RPT.cs/TXEmail.cs
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/30055_1.xlsx
+++ b/PhoenixCI/Excel_Template/30055_1.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJSOFT\Source\Workspaces\PhoenixCI\PhoenixCI_Kj\PhoenixCI\Excel_Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vs\PhoenixCI_Kj\PhoenixCI\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE84DE45-C68A-4775-9024-B62BB4320452}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D165DC50-D83E-4D6A-80AD-4729FF4C8EC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="商品期貨看板" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="124">
   <si>
     <t>漲跌</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -682,12 +683,39 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>漲跌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>契約名稱</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品期貨看板</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>黃金(美元)</t>
+  </si>
+  <si>
+    <t>黃金(臺幣)</t>
+  </si>
+  <si>
+    <t>布蘭特原油</t>
+  </si>
+  <si>
+    <t>註：近月合約每日結算價</t>
+  </si>
+  <si>
+    <t>價格</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="8">
+  <numFmts count="10">
     <numFmt numFmtId="176" formatCode="0.00_ ;[Red]\-0.00\ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="General;;\-"/>
@@ -696,8 +724,10 @@
     <numFmt numFmtId="185" formatCode="#,##0_ "/>
     <numFmt numFmtId="187" formatCode="0.0000_ "/>
     <numFmt numFmtId="189" formatCode="0.0"/>
+    <numFmt numFmtId="193" formatCode="0.00;\-0.00;\-;@\ "/>
+    <numFmt numFmtId="194" formatCode="0.0000;\-0.0000;\-;@\ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -910,6 +940,20 @@
       <name val="標楷體"/>
       <family val="4"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="29">
@@ -1274,7 +1318,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1332,6 +1376,9 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1402,7 +1449,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1616,6 +1663,36 @@
     <xf numFmtId="189" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="189" fontId="25" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="189" fontId="25" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="193" fontId="22" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="194" fontId="28" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1727,8 +1804,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - 輔色1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - 輔色2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - 輔色3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -1748,29 +1831,30 @@
     <cellStyle name="60% - 輔色5" xfId="17" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - 輔色6" xfId="18" builtinId="52" customBuiltin="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="中等" xfId="19" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="合計" xfId="20" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="好" xfId="21" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="計算方式" xfId="22" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="連結的儲存格" xfId="23" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="備註" xfId="24" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="說明文字" xfId="25" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="輔色1" xfId="26" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="輔色2" xfId="27" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="輔色3" xfId="28" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="輔色4" xfId="29" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="輔色5" xfId="30" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="輔色6" xfId="31" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="標題" xfId="32" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="標題 1" xfId="33" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="標題 2" xfId="34" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="標題 3" xfId="35" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="標題 4" xfId="36" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="輸入" xfId="37" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="輸出" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="檢查儲存格" xfId="39" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="壞" xfId="40" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="警告文字" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="一般 2" xfId="19"/>
+    <cellStyle name="中等" xfId="20" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="合計" xfId="21" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="好" xfId="22" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="計算方式" xfId="23" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="連結的儲存格" xfId="24" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="備註" xfId="25" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="說明文字" xfId="26" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="輔色1" xfId="27" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="輔色2" xfId="28" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="輔色3" xfId="29" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="輔色4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="輔色5" xfId="31" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="輔色6" xfId="32" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="標題" xfId="33" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="標題 1" xfId="34" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="標題 2" xfId="35" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="標題 3" xfId="36" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="標題 4" xfId="37" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="輸入" xfId="38" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="輸出" xfId="39" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="檢查儲存格" xfId="40" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="壞" xfId="41" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="警告文字" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2112,13 +2196,15 @@
   </sheetPr>
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S149" sqref="S149"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123:J134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="5" width="9" style="26"/>
+    <col min="1" max="3" width="9" style="26"/>
+    <col min="4" max="4" width="10.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="26"/>
     <col min="6" max="6" width="12.875" style="26" customWidth="1"/>
     <col min="7" max="9" width="9" style="26"/>
     <col min="10" max="10" width="9.5" style="26" customWidth="1"/>
@@ -2146,11 +2232,11 @@
       <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="102"/>
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:9">
@@ -2495,10 +2581,10 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="21">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="98"/>
+      <c r="B31" s="108"/>
       <c r="C31" s="51" t="s">
         <v>37</v>
       </c>
@@ -2516,10 +2602,10 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="84" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2531,8 +2617,8 @@
       <c r="G32" s="53"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="93"/>
-      <c r="B33" s="93"/>
+      <c r="A33" s="103"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="3" t="s">
         <v>9</v>
       </c>
@@ -2542,8 +2628,8 @@
       <c r="G33" s="53"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="93"/>
-      <c r="B34" s="88"/>
+      <c r="A34" s="103"/>
+      <c r="B34" s="98"/>
       <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
@@ -2553,8 +2639,8 @@
       <c r="G34" s="53"/>
     </row>
     <row r="35" spans="1:7" ht="21">
-      <c r="A35" s="94"/>
-      <c r="B35" s="74" t="s">
+      <c r="A35" s="104"/>
+      <c r="B35" s="84" t="s">
         <v>51</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2566,8 +2652,8 @@
       <c r="G35" s="53"/>
     </row>
     <row r="36" spans="1:7" ht="21">
-      <c r="A36" s="75"/>
-      <c r="B36" s="75"/>
+      <c r="A36" s="85"/>
+      <c r="B36" s="85"/>
       <c r="C36" s="3" t="s">
         <v>30</v>
       </c>
@@ -2577,10 +2663,10 @@
       <c r="G36" s="53"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" hidden="1" customHeight="1">
-      <c r="A37" s="74" t="s">
+      <c r="A37" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="74" t="s">
+      <c r="B37" s="84" t="s">
         <v>17</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2592,8 +2678,8 @@
       <c r="G37" s="53"/>
     </row>
     <row r="38" spans="1:7" hidden="1">
-      <c r="A38" s="93"/>
-      <c r="B38" s="93"/>
+      <c r="A38" s="103"/>
+      <c r="B38" s="103"/>
       <c r="C38" s="3" t="s">
         <v>9</v>
       </c>
@@ -2603,8 +2689,8 @@
       <c r="G38" s="53"/>
     </row>
     <row r="39" spans="1:7" ht="16.5" hidden="1" customHeight="1">
-      <c r="A39" s="93"/>
-      <c r="B39" s="88"/>
+      <c r="A39" s="103"/>
+      <c r="B39" s="98"/>
       <c r="C39" s="3" t="s">
         <v>10</v>
       </c>
@@ -2614,8 +2700,8 @@
       <c r="G39" s="53"/>
     </row>
     <row r="40" spans="1:7" ht="21" hidden="1">
-      <c r="A40" s="94"/>
-      <c r="B40" s="74" t="s">
+      <c r="A40" s="104"/>
+      <c r="B40" s="84" t="s">
         <v>22</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2627,8 +2713,8 @@
       <c r="G40" s="53"/>
     </row>
     <row r="41" spans="1:7" ht="21" hidden="1">
-      <c r="A41" s="75"/>
-      <c r="B41" s="88"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="98"/>
       <c r="C41" s="3" t="s">
         <v>30</v>
       </c>
@@ -2638,10 +2724,10 @@
       <c r="G41" s="53"/>
     </row>
     <row r="42" spans="1:7" hidden="1">
-      <c r="A42" s="74" t="s">
+      <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="76" t="s">
+      <c r="B42" s="86" t="s">
         <v>21</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -2653,8 +2739,8 @@
       <c r="G42" s="53"/>
     </row>
     <row r="43" spans="1:7" hidden="1">
-      <c r="A43" s="93"/>
-      <c r="B43" s="77"/>
+      <c r="A43" s="103"/>
+      <c r="B43" s="87"/>
       <c r="C43" s="3" t="s">
         <v>9</v>
       </c>
@@ -2664,8 +2750,8 @@
       <c r="G43" s="53"/>
     </row>
     <row r="44" spans="1:7" hidden="1">
-      <c r="A44" s="93"/>
-      <c r="B44" s="78"/>
+      <c r="A44" s="103"/>
+      <c r="B44" s="88"/>
       <c r="C44" s="3" t="s">
         <v>10</v>
       </c>
@@ -2675,8 +2761,8 @@
       <c r="G44" s="53"/>
     </row>
     <row r="45" spans="1:7" ht="21" hidden="1">
-      <c r="A45" s="94"/>
-      <c r="B45" s="76" t="s">
+      <c r="A45" s="104"/>
+      <c r="B45" s="86" t="s">
         <v>16</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2688,8 +2774,8 @@
       <c r="G45" s="53"/>
     </row>
     <row r="46" spans="1:7" ht="21" hidden="1">
-      <c r="A46" s="75"/>
-      <c r="B46" s="78"/>
+      <c r="A46" s="85"/>
+      <c r="B46" s="88"/>
       <c r="C46" s="3" t="s">
         <v>30</v>
       </c>
@@ -2706,23 +2792,23 @@
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="82"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="103" t="s">
+      <c r="B49" s="92"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="92"/>
+      <c r="E49" s="92"/>
+      <c r="F49" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="G49" s="81" t="s">
+      <c r="G49" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="82"/>
-      <c r="I49" s="82"/>
-      <c r="J49" s="82"/>
-      <c r="K49" s="83"/>
+      <c r="H49" s="92"/>
+      <c r="I49" s="92"/>
+      <c r="J49" s="92"/>
+      <c r="K49" s="93"/>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="3" t="s">
@@ -2740,7 +2826,7 @@
       <c r="E50" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F50" s="75"/>
+      <c r="F50" s="85"/>
       <c r="G50" s="3" t="s">
         <v>23</v>
       </c>
@@ -2981,23 +3067,23 @@
       <c r="D66" s="9"/>
     </row>
     <row r="67" spans="1:11" s="43" customFormat="1" ht="16.5" hidden="1" customHeight="1">
-      <c r="A67" s="81" t="s">
+      <c r="A67" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="82"/>
-      <c r="C67" s="82"/>
-      <c r="D67" s="82"/>
-      <c r="E67" s="83"/>
-      <c r="F67" s="99" t="s">
+      <c r="B67" s="92"/>
+      <c r="C67" s="92"/>
+      <c r="D67" s="92"/>
+      <c r="E67" s="93"/>
+      <c r="F67" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="G67" s="81" t="s">
+      <c r="G67" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="H67" s="82"/>
-      <c r="I67" s="82"/>
-      <c r="J67" s="82"/>
-      <c r="K67" s="83"/>
+      <c r="H67" s="92"/>
+      <c r="I67" s="92"/>
+      <c r="J67" s="92"/>
+      <c r="K67" s="93"/>
     </row>
     <row r="68" spans="1:11" s="43" customFormat="1" hidden="1">
       <c r="A68" s="3" t="s">
@@ -3015,7 +3101,7 @@
       <c r="E68" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F68" s="100"/>
+      <c r="F68" s="110"/>
       <c r="G68" s="3" t="s">
         <v>23</v>
       </c>
@@ -3119,24 +3205,24 @@
       <c r="F75" s="2"/>
     </row>
     <row r="76" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A76" s="74" t="s">
+      <c r="A76" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="95" t="s">
+      <c r="B76" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="C76" s="96"/>
-      <c r="D76" s="96"/>
-      <c r="E76" s="97"/>
-      <c r="F76" s="81" t="s">
+      <c r="C76" s="106"/>
+      <c r="D76" s="106"/>
+      <c r="E76" s="107"/>
+      <c r="F76" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="G76" s="82"/>
-      <c r="H76" s="82"/>
-      <c r="I76" s="83"/>
+      <c r="G76" s="92"/>
+      <c r="H76" s="92"/>
+      <c r="I76" s="93"/>
     </row>
     <row r="77" spans="1:11" ht="21">
-      <c r="A77" s="75"/>
+      <c r="A77" s="85"/>
       <c r="B77" s="37" t="s">
         <v>5</v>
       </c>
@@ -3309,12 +3395,12 @@
       <c r="A90" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B90" s="101" t="s">
+      <c r="B90" s="111" t="s">
         <v>109</v>
       </c>
-      <c r="C90" s="102"/>
-      <c r="D90" s="102"/>
-      <c r="E90" s="102"/>
+      <c r="C90" s="112"/>
+      <c r="D90" s="112"/>
+      <c r="E90" s="112"/>
     </row>
     <row r="91" spans="1:10" ht="31.5">
       <c r="A91" s="3" t="s">
@@ -3401,24 +3487,24 @@
       <c r="I96" s="7"/>
     </row>
     <row r="98" spans="1:12" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A98" s="85" t="s">
+      <c r="A98" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="B98" s="85"/>
-      <c r="C98" s="85"/>
-      <c r="D98" s="85"/>
-      <c r="E98" s="85"/>
-      <c r="F98" s="85"/>
-      <c r="G98" s="85"/>
-      <c r="H98" s="85"/>
-      <c r="I98" s="87"/>
-      <c r="J98" s="87"/>
+      <c r="B98" s="95"/>
+      <c r="C98" s="95"/>
+      <c r="D98" s="95"/>
+      <c r="E98" s="95"/>
+      <c r="F98" s="95"/>
+      <c r="G98" s="95"/>
+      <c r="H98" s="95"/>
+      <c r="I98" s="97"/>
+      <c r="J98" s="97"/>
     </row>
     <row r="99" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A99" s="79" t="s">
+      <c r="A99" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="B99" s="84"/>
+      <c r="B99" s="94"/>
       <c r="C99" s="17" t="s">
         <v>72</v>
       </c>
@@ -3445,112 +3531,112 @@
       </c>
     </row>
     <row r="100" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A100" s="79"/>
-      <c r="B100" s="84"/>
+      <c r="A100" s="89"/>
+      <c r="B100" s="94"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
+      <c r="D100" s="79"/>
+      <c r="E100" s="79"/>
       <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
+      <c r="G100" s="79"/>
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
     </row>
     <row r="101" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A101" s="79"/>
-      <c r="B101" s="84"/>
+      <c r="A101" s="89"/>
+      <c r="B101" s="94"/>
       <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
+      <c r="D101" s="79"/>
+      <c r="E101" s="79"/>
       <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
+      <c r="G101" s="79"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
     </row>
     <row r="102" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A102" s="79"/>
-      <c r="B102" s="84"/>
+      <c r="A102" s="89"/>
+      <c r="B102" s="94"/>
       <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
+      <c r="D102" s="79"/>
+      <c r="E102" s="79"/>
       <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
+      <c r="G102" s="79"/>
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
     </row>
     <row r="103" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A103" s="79"/>
-      <c r="B103" s="80"/>
+      <c r="A103" s="89"/>
+      <c r="B103" s="90"/>
       <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
+      <c r="D103" s="79"/>
+      <c r="E103" s="79"/>
       <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
+      <c r="G103" s="79"/>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
     </row>
     <row r="104" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A104" s="79"/>
-      <c r="B104" s="84"/>
+      <c r="A104" s="89"/>
+      <c r="B104" s="94"/>
       <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
+      <c r="D104" s="79"/>
+      <c r="E104" s="79"/>
       <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
+      <c r="G104" s="79"/>
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
     </row>
     <row r="105" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A105" s="72"/>
-      <c r="B105" s="73"/>
+      <c r="A105" s="82"/>
+      <c r="B105" s="83"/>
       <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
+      <c r="D105" s="79"/>
+      <c r="E105" s="79"/>
       <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
+      <c r="G105" s="79"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
     </row>
     <row r="106" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A106" s="72"/>
-      <c r="B106" s="73"/>
+      <c r="A106" s="82"/>
+      <c r="B106" s="83"/>
       <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
+      <c r="D106" s="79"/>
+      <c r="E106" s="79"/>
       <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
+      <c r="G106" s="79"/>
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
     </row>
     <row r="107" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A107" s="72"/>
-      <c r="B107" s="73"/>
+      <c r="A107" s="82"/>
+      <c r="B107" s="83"/>
       <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
+      <c r="D107" s="79"/>
+      <c r="E107" s="79"/>
       <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
+      <c r="G107" s="79"/>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
     </row>
     <row r="108" spans="1:12" s="16" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A108" s="20"/>
-      <c r="B108" s="20"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="21"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="21"/>
-      <c r="H108" s="21"/>
-      <c r="I108" s="22"/>
-      <c r="J108" s="22"/>
+      <c r="A108" s="82"/>
+      <c r="B108" s="83"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="79"/>
+      <c r="E108" s="79"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="79"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
     </row>
     <row r="109" spans="1:12" s="16" customFormat="1" hidden="1">
       <c r="A109" s="26"/>
@@ -3568,26 +3654,26 @@
       <c r="K109" s="26"/>
     </row>
     <row r="110" spans="1:12" s="16" customFormat="1" hidden="1">
-      <c r="A110" s="81" t="s">
+      <c r="A110" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B110" s="82"/>
-      <c r="C110" s="82"/>
-      <c r="D110" s="82"/>
-      <c r="E110" s="82"/>
-      <c r="F110" s="104" t="s">
+      <c r="B110" s="92"/>
+      <c r="C110" s="92"/>
+      <c r="D110" s="92"/>
+      <c r="E110" s="92"/>
+      <c r="F110" s="114" t="s">
         <v>87</v>
       </c>
-      <c r="G110" s="104" t="s">
+      <c r="G110" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="H110" s="81" t="s">
+      <c r="H110" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="I110" s="82"/>
-      <c r="J110" s="82"/>
-      <c r="K110" s="82"/>
-      <c r="L110" s="83"/>
+      <c r="I110" s="92"/>
+      <c r="J110" s="92"/>
+      <c r="K110" s="92"/>
+      <c r="L110" s="93"/>
     </row>
     <row r="111" spans="1:12" s="16" customFormat="1" hidden="1">
       <c r="A111" s="3" t="s">
@@ -3605,8 +3691,8 @@
       <c r="E111" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="F111" s="105"/>
-      <c r="G111" s="106"/>
+      <c r="F111" s="115"/>
+      <c r="G111" s="116"/>
       <c r="H111" s="3" t="s">
         <v>23</v>
       </c>
@@ -3736,7 +3822,7 @@
       <c r="K119" s="34"/>
       <c r="L119" s="54"/>
     </row>
-    <row r="120" spans="1:13" s="16" customFormat="1" ht="18.75" hidden="1" customHeight="1">
+    <row r="120" spans="1:13" s="16" customFormat="1" ht="18.75" customHeight="1">
       <c r="A120" s="20"/>
       <c r="B120" s="20"/>
       <c r="C120" s="21"/>
@@ -3749,16 +3835,16 @@
       <c r="J120" s="22"/>
     </row>
     <row r="121" spans="1:13" s="16" customFormat="1">
-      <c r="A121" s="85" t="s">
+      <c r="A121" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="B121" s="85"/>
-      <c r="C121" s="85"/>
-      <c r="D121" s="85"/>
-      <c r="E121" s="85"/>
-      <c r="F121" s="85"/>
-      <c r="G121" s="85"/>
-      <c r="H121" s="85"/>
+      <c r="B121" s="95"/>
+      <c r="C121" s="95"/>
+      <c r="D121" s="95"/>
+      <c r="E121" s="95"/>
+      <c r="F121" s="95"/>
+      <c r="G121" s="95"/>
+      <c r="H121" s="95"/>
       <c r="I121" s="6"/>
       <c r="J121" s="6"/>
       <c r="L121" s="16" t="s">
@@ -3766,10 +3852,10 @@
       </c>
     </row>
     <row r="122" spans="1:13" s="16" customFormat="1">
-      <c r="A122" s="79" t="s">
+      <c r="A122" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="B122" s="84"/>
+      <c r="B122" s="94"/>
       <c r="C122" s="17" t="s">
         <v>81</v>
       </c>
@@ -3796,181 +3882,181 @@
       </c>
     </row>
     <row r="123" spans="1:13" s="16" customFormat="1">
-      <c r="A123" s="74" t="s">
+      <c r="A123" s="84" t="s">
         <v>82</v>
       </c>
       <c r="B123" s="23" t="s">
         <v>83</v>
       </c>
       <c r="C123" s="24"/>
-      <c r="D123" s="24"/>
-      <c r="E123" s="24"/>
+      <c r="D123" s="80"/>
+      <c r="E123" s="80"/>
       <c r="F123" s="24"/>
-      <c r="G123" s="24"/>
+      <c r="G123" s="80"/>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
     </row>
     <row r="124" spans="1:13" s="16" customFormat="1">
-      <c r="A124" s="88"/>
+      <c r="A124" s="98"/>
       <c r="B124" s="23" t="s">
         <v>84</v>
       </c>
       <c r="C124" s="24"/>
-      <c r="D124" s="24"/>
-      <c r="E124" s="24"/>
+      <c r="D124" s="80"/>
+      <c r="E124" s="80"/>
       <c r="F124" s="24"/>
-      <c r="G124" s="24"/>
+      <c r="G124" s="80"/>
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
     </row>
     <row r="125" spans="1:13" s="16" customFormat="1">
-      <c r="A125" s="74" t="s">
+      <c r="A125" s="84" t="s">
         <v>85</v>
       </c>
       <c r="B125" s="23" t="s">
         <v>83</v>
       </c>
       <c r="C125" s="24"/>
-      <c r="D125" s="24"/>
-      <c r="E125" s="24"/>
+      <c r="D125" s="80"/>
+      <c r="E125" s="80"/>
       <c r="F125" s="24"/>
-      <c r="G125" s="24"/>
+      <c r="G125" s="80"/>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
     </row>
     <row r="126" spans="1:13" s="16" customFormat="1">
-      <c r="A126" s="88"/>
+      <c r="A126" s="98"/>
       <c r="B126" s="23" t="s">
         <v>84</v>
       </c>
       <c r="C126" s="24"/>
-      <c r="D126" s="24"/>
-      <c r="E126" s="24"/>
+      <c r="D126" s="80"/>
+      <c r="E126" s="80"/>
       <c r="F126" s="24"/>
-      <c r="G126" s="24"/>
+      <c r="G126" s="80"/>
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
     </row>
     <row r="127" spans="1:13" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A127" s="74" t="s">
+      <c r="A127" s="84" t="s">
         <v>93</v>
       </c>
       <c r="B127" s="23" t="s">
         <v>83</v>
       </c>
       <c r="C127" s="24"/>
-      <c r="D127" s="24"/>
-      <c r="E127" s="24"/>
+      <c r="D127" s="80"/>
+      <c r="E127" s="80"/>
       <c r="F127" s="24"/>
-      <c r="G127" s="24"/>
+      <c r="G127" s="80"/>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
     </row>
     <row r="128" spans="1:13" s="16" customFormat="1">
-      <c r="A128" s="88"/>
+      <c r="A128" s="98"/>
       <c r="B128" s="23" t="s">
         <v>84</v>
       </c>
       <c r="C128" s="24"/>
-      <c r="D128" s="24"/>
-      <c r="E128" s="24"/>
+      <c r="D128" s="80"/>
+      <c r="E128" s="80"/>
       <c r="F128" s="24"/>
-      <c r="G128" s="24"/>
+      <c r="G128" s="80"/>
       <c r="H128" s="7"/>
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
     </row>
     <row r="129" spans="1:12" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A129" s="74" t="s">
+      <c r="A129" s="84" t="s">
         <v>94</v>
       </c>
       <c r="B129" s="23" t="s">
         <v>83</v>
       </c>
       <c r="C129" s="24"/>
-      <c r="D129" s="24"/>
-      <c r="E129" s="24"/>
+      <c r="D129" s="80"/>
+      <c r="E129" s="80"/>
       <c r="F129" s="24"/>
-      <c r="G129" s="24"/>
+      <c r="G129" s="80"/>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
     </row>
     <row r="130" spans="1:12" s="16" customFormat="1">
-      <c r="A130" s="88"/>
+      <c r="A130" s="98"/>
       <c r="B130" s="23" t="s">
         <v>84</v>
       </c>
       <c r="C130" s="24"/>
-      <c r="D130" s="24"/>
-      <c r="E130" s="24"/>
+      <c r="D130" s="80"/>
+      <c r="E130" s="80"/>
       <c r="F130" s="24"/>
-      <c r="G130" s="24"/>
+      <c r="G130" s="80"/>
       <c r="H130" s="7"/>
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
     </row>
     <row r="131" spans="1:12" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A131" s="74" t="s">
+      <c r="A131" s="84" t="s">
         <v>99</v>
       </c>
       <c r="B131" s="23" t="s">
         <v>100</v>
       </c>
       <c r="C131" s="24"/>
-      <c r="D131" s="24"/>
-      <c r="E131" s="24"/>
+      <c r="D131" s="80"/>
+      <c r="E131" s="80"/>
       <c r="F131" s="24"/>
-      <c r="G131" s="24"/>
+      <c r="G131" s="80"/>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
     </row>
     <row r="132" spans="1:12" s="16" customFormat="1">
-      <c r="A132" s="75"/>
+      <c r="A132" s="85"/>
       <c r="B132" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C132" s="24"/>
-      <c r="D132" s="24"/>
-      <c r="E132" s="24"/>
+      <c r="D132" s="80"/>
+      <c r="E132" s="80"/>
       <c r="F132" s="24"/>
-      <c r="G132" s="24"/>
+      <c r="G132" s="80"/>
       <c r="H132" s="7"/>
       <c r="I132" s="7"/>
       <c r="J132" s="7"/>
     </row>
     <row r="133" spans="1:12" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A133" s="74" t="s">
+      <c r="A133" s="84" t="s">
         <v>102</v>
       </c>
       <c r="B133" s="23" t="s">
         <v>100</v>
       </c>
       <c r="C133" s="24"/>
-      <c r="D133" s="24"/>
-      <c r="E133" s="24"/>
+      <c r="D133" s="80"/>
+      <c r="E133" s="80"/>
       <c r="F133" s="24"/>
-      <c r="G133" s="24"/>
+      <c r="G133" s="80"/>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
     </row>
     <row r="134" spans="1:12" s="16" customFormat="1">
-      <c r="A134" s="88"/>
+      <c r="A134" s="98"/>
       <c r="B134" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C134" s="24"/>
-      <c r="D134" s="24"/>
-      <c r="E134" s="24"/>
+      <c r="D134" s="80"/>
+      <c r="E134" s="80"/>
       <c r="F134" s="24"/>
-      <c r="G134" s="24"/>
+      <c r="G134" s="80"/>
       <c r="H134" s="7"/>
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
@@ -3979,39 +4065,39 @@
     <row r="136" spans="1:12" s="16" customFormat="1" hidden="1">
       <c r="A136" s="26"/>
       <c r="B136" s="2"/>
-      <c r="C136" s="107" t="s">
+      <c r="C136" s="117" t="s">
         <v>90</v>
       </c>
-      <c r="D136" s="102"/>
-      <c r="E136" s="102"/>
-      <c r="F136" s="102"/>
-      <c r="G136" s="102"/>
+      <c r="D136" s="112"/>
+      <c r="E136" s="112"/>
+      <c r="F136" s="112"/>
+      <c r="G136" s="112"/>
       <c r="H136" s="26"/>
       <c r="I136" s="26"/>
       <c r="J136" s="26"/>
       <c r="K136" s="26"/>
     </row>
     <row r="137" spans="1:12" s="16" customFormat="1" hidden="1">
-      <c r="A137" s="81" t="s">
+      <c r="A137" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B137" s="82"/>
-      <c r="C137" s="82"/>
-      <c r="D137" s="82"/>
-      <c r="E137" s="82"/>
-      <c r="F137" s="104" t="s">
+      <c r="B137" s="92"/>
+      <c r="C137" s="92"/>
+      <c r="D137" s="92"/>
+      <c r="E137" s="92"/>
+      <c r="F137" s="114" t="s">
         <v>87</v>
       </c>
-      <c r="G137" s="104" t="s">
+      <c r="G137" s="114" t="s">
         <v>60</v>
       </c>
-      <c r="H137" s="81" t="s">
+      <c r="H137" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="I137" s="82"/>
-      <c r="J137" s="82"/>
-      <c r="K137" s="82"/>
-      <c r="L137" s="83"/>
+      <c r="I137" s="92"/>
+      <c r="J137" s="92"/>
+      <c r="K137" s="92"/>
+      <c r="L137" s="93"/>
     </row>
     <row r="138" spans="1:12" s="16" customFormat="1" hidden="1">
       <c r="A138" s="3" t="s">
@@ -4029,8 +4115,8 @@
       <c r="E138" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="F138" s="105"/>
-      <c r="G138" s="106"/>
+      <c r="F138" s="115"/>
+      <c r="G138" s="116"/>
       <c r="H138" s="3" t="s">
         <v>23</v>
       </c>
@@ -4104,24 +4190,24 @@
       <c r="L142" s="59"/>
     </row>
     <row r="143" spans="1:12">
-      <c r="A143" s="85" t="s">
+      <c r="A143" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="B143" s="85"/>
-      <c r="C143" s="85"/>
-      <c r="D143" s="85"/>
-      <c r="E143" s="85"/>
-      <c r="F143" s="85"/>
-      <c r="G143" s="85"/>
-      <c r="H143" s="85"/>
+      <c r="B143" s="95"/>
+      <c r="C143" s="95"/>
+      <c r="D143" s="95"/>
+      <c r="E143" s="95"/>
+      <c r="F143" s="95"/>
+      <c r="G143" s="95"/>
+      <c r="H143" s="95"/>
       <c r="K143" s="58"/>
       <c r="L143" s="59"/>
     </row>
     <row r="144" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A144" s="79" t="s">
+      <c r="A144" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="B144" s="84"/>
+      <c r="B144" s="94"/>
       <c r="C144" s="17" t="s">
         <v>23</v>
       </c>
@@ -4150,7 +4236,7 @@
       <c r="L144" s="59"/>
     </row>
     <row r="145" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A145" s="71" t="s">
+      <c r="A145" s="81" t="s">
         <v>113</v>
       </c>
       <c r="B145" s="23" t="s">
@@ -4168,7 +4254,7 @@
       <c r="L145" s="59"/>
     </row>
     <row r="146" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A146" s="71"/>
+      <c r="A146" s="81"/>
       <c r="B146" s="23" t="s">
         <v>105</v>
       </c>
@@ -4184,7 +4270,7 @@
       <c r="L146" s="59"/>
     </row>
     <row r="147" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A147" s="71" t="s">
+      <c r="A147" s="81" t="s">
         <v>107</v>
       </c>
       <c r="B147" s="23" t="s">
@@ -4202,7 +4288,7 @@
       <c r="L147" s="59"/>
     </row>
     <row r="148" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A148" s="71"/>
+      <c r="A148" s="81"/>
       <c r="B148" s="23" t="s">
         <v>105</v>
       </c>
@@ -4218,7 +4304,7 @@
       <c r="L148" s="59"/>
     </row>
     <row r="149" spans="1:12" ht="21" customHeight="1">
-      <c r="A149" s="89" t="s">
+      <c r="A149" s="99" t="s">
         <v>104</v>
       </c>
       <c r="B149" s="23" t="s">
@@ -4236,7 +4322,7 @@
       <c r="L149" s="59"/>
     </row>
     <row r="150" spans="1:12">
-      <c r="A150" s="89"/>
+      <c r="A150" s="99"/>
       <c r="B150" s="23" t="s">
         <v>105</v>
       </c>
@@ -4266,18 +4352,18 @@
       <c r="L151" s="59"/>
     </row>
     <row r="152" spans="1:12">
-      <c r="A152" s="86" t="s">
+      <c r="A152" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="B152" s="86"/>
-      <c r="C152" s="86"/>
-      <c r="D152" s="86"/>
-      <c r="E152" s="86"/>
-      <c r="F152" s="86"/>
-      <c r="G152" s="86"/>
-      <c r="H152" s="86"/>
-      <c r="I152" s="86"/>
-      <c r="J152" s="86"/>
+      <c r="B152" s="96"/>
+      <c r="C152" s="96"/>
+      <c r="D152" s="96"/>
+      <c r="E152" s="96"/>
+      <c r="F152" s="96"/>
+      <c r="G152" s="96"/>
+      <c r="H152" s="96"/>
+      <c r="I152" s="96"/>
+      <c r="J152" s="96"/>
       <c r="L152" s="66"/>
     </row>
     <row r="153" spans="1:12">
@@ -4323,7 +4409,7 @@
       <c r="J155" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="56">
     <mergeCell ref="C136:G136"/>
     <mergeCell ref="H137:L137"/>
     <mergeCell ref="A110:E110"/>
@@ -4342,6 +4428,7 @@
     <mergeCell ref="A127:A128"/>
     <mergeCell ref="A121:H121"/>
     <mergeCell ref="G110:G111"/>
+    <mergeCell ref="A108:B108"/>
     <mergeCell ref="B90:E90"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="B32:B34"/>
@@ -4475,4 +4562,124 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E1:E65536"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="1.125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="119" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="119"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="71">
+        <f>Sheet1!F145</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="72">
+        <f>Sheet1!G145</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="73" t="str">
+        <f>IF(C3&lt;0,"↓",IF(C3&gt;0,"↑",""))</f>
+        <v/>
+      </c>
+      <c r="E3" s="74">
+        <f>ABS(C3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="76" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="71">
+        <f>Sheet1!F147</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="72">
+        <f>Sheet1!G147</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="73" t="str">
+        <f>IF(C4&lt;0,"↓",IF(C4&gt;0,"↑",""))</f>
+        <v/>
+      </c>
+      <c r="E4" s="74">
+        <f>ABS(C4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="72">
+        <f>Sheet1!F149</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="72">
+        <f>Sheet1!G149</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="73" t="str">
+        <f>IF(C5&lt;0,"↓",IF(C5&gt;0,"↑",""))</f>
+        <v/>
+      </c>
+      <c r="E5" s="74">
+        <f>ABS(C5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>